<commit_message>
correccion de bug en requisicion y xlsx de inventariocierresemana
</commit_message>
<xml_diff>
--- a/public/application/files/jasper/templates/inventariocierresemana.xlsx
+++ b/public/application/files/jasper/templates/inventariocierresemana.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>{compania:nombre}</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>{col:dieciocho}</t>
+  </si>
+  <si>
+    <t>{compania:sucursal}</t>
+  </si>
+  <si>
+    <t>{compania:almacen}</t>
   </si>
 </sst>
 </file>
@@ -217,8 +223,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -271,7 +281,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -283,6 +293,8 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -294,6 +306,8 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -623,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="W11" sqref="W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -660,135 +674,103 @@
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
     </row>
-    <row r="2" spans="1:18" ht="18">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:18" ht="28">
+      <c r="A2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+    </row>
+    <row r="3" spans="1:18" ht="28">
+      <c r="A3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+    </row>
+    <row r="4" spans="1:18" ht="18">
+      <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-    </row>
-    <row r="3" spans="1:18">
-      <c r="A3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="9"/>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="9"/>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -802,15 +784,94 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A4:F4"/>
+  <mergeCells count="6">
+    <mergeCell ref="A6:F6"/>
     <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A4:R4"/>
+    <mergeCell ref="B5:R5"/>
+    <mergeCell ref="A3:R3"/>
     <mergeCell ref="A2:R2"/>
-    <mergeCell ref="B3:R3"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>